<commit_message>
update database + title and logo
</commit_message>
<xml_diff>
--- a/src/components/database/database.xlsx
+++ b/src/components/database/database.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\userPC\Desktop\PizzaLand\pizza-land\src\components\database\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\userPC\Desktop\PizzaLand_PUBLICK\PizzaLand\src\components\database\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{015642CE-3990-4C66-9A70-2C682B62E3EC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{11310DBA-E31E-4901-B26C-55C8B010DB47}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="pizzas" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="74">
   <si>
     <t>ID</t>
   </si>
@@ -98,9 +98,6 @@
     <t>Salad5</t>
   </si>
   <si>
-    <t>https://idsb.tmgrup.com.tr/ly/uploads/images/2023/01/15/251807.jpg</t>
-  </si>
-  <si>
     <t>https://src.zakaz.atbmarket.com/cache/photos/37541/catalog_list_37541.jpg</t>
   </si>
   <si>
@@ -110,9 +107,6 @@
     <t>sizes</t>
   </si>
   <si>
-    <t>50;100;150</t>
-  </si>
-  <si>
     <t>50;100</t>
   </si>
   <si>
@@ -146,46 +140,124 @@
     <t>city</t>
   </si>
   <si>
-    <t>ny1</t>
-  </si>
-  <si>
-    <t>ny2</t>
-  </si>
-  <si>
-    <t>ny3</t>
-  </si>
-  <si>
-    <t>lviv1</t>
-  </si>
-  <si>
-    <t>kiyv1</t>
-  </si>
-  <si>
-    <t>lviv2</t>
-  </si>
-  <si>
-    <t>lviv3</t>
-  </si>
-  <si>
-    <t>lviv4</t>
-  </si>
-  <si>
-    <t>kiyv2</t>
-  </si>
-  <si>
-    <t>Drink1</t>
-  </si>
-  <si>
-    <t>Drink2</t>
-  </si>
-  <si>
-    <t>Drink3</t>
-  </si>
-  <si>
-    <t>Drink4</t>
-  </si>
-  <si>
-    <t>Drink5</t>
+    <t>Novoyavorivsk Pizzeria №1</t>
+  </si>
+  <si>
+    <t>Novoyavorivsk Pizzeria №2</t>
+  </si>
+  <si>
+    <t>Novoyavorivsk Pizzeria №3</t>
+  </si>
+  <si>
+    <t>Lviv Pizzeria №1</t>
+  </si>
+  <si>
+    <t>Lviv Pizzeria №2</t>
+  </si>
+  <si>
+    <t>Lviv Pizzeria №3</t>
+  </si>
+  <si>
+    <t>Lviv Pizzeria №4</t>
+  </si>
+  <si>
+    <t>Kiyv Pizzeria №1</t>
+  </si>
+  <si>
+    <t>Kiyv Pizzeria №2</t>
+  </si>
+  <si>
+    <t>https://encrypted-tbn0.gstatic.com/images?q=tbn:ANd9GcRwqT-NA50cbZnRpVHfAWurrMld20hAub4xUg&amp;usqp=CAU</t>
+  </si>
+  <si>
+    <t>https://foodcom.pl/wp-content/uploads/2023/02/coca-cola-min.png</t>
+  </si>
+  <si>
+    <t>https://icf.listex.info/med/44c7c387-35ae-29a5-ab08-8c7ab661e71e.jpg</t>
+  </si>
+  <si>
+    <t>https://zakaz.idealmarket.net.ua/images/virtuemart/product/129284.jpg</t>
+  </si>
+  <si>
+    <t>50;70</t>
+  </si>
+  <si>
+    <t>1l;5l</t>
+  </si>
+  <si>
+    <t>Volya</t>
+  </si>
+  <si>
+    <t>Mohito</t>
+  </si>
+  <si>
+    <t>Coca Cola</t>
+  </si>
+  <si>
+    <t>Pepsi</t>
+  </si>
+  <si>
+    <t>Zhivchik</t>
+  </si>
+  <si>
+    <t>https://cdn.loveandlemons.com/wp-content/uploads/2021/04/green-salad.jpg</t>
+  </si>
+  <si>
+    <t>https://www.eatingwell.com/thmb/Qcd3ZdtD608IfSDyax6AFvZrj-0=/1500x0/filters:no_upscale():max_bytes(150000):strip_icc()/Eat-the-Rainbow-Chopped-Salad-with-Basil-Mozzarella-4f304ec0564944f98016b36765124667.jpg</t>
+  </si>
+  <si>
+    <t>https://lh3.googleusercontent.com/3bAa3OYBGhjPd3zUYTvwAQhMWZ_mju0GE8S7pj6ly7c3qxm34KwRw5-WUlx8dpNvLXndfMfxC2na1qODYLSQ3w=w1300-h1300-c-rj-v1-e365</t>
+  </si>
+  <si>
+    <t>https://saladswithanastasia.com/wp-content/uploads/2021/12/radish-green-salad-land1.jpg</t>
+  </si>
+  <si>
+    <t>https://www.tablefortwoblog.com/wp-content/uploads/2018/05/quick-chopped-salad-recipe-photos-tablefortwoblog-3.jpg</t>
+  </si>
+  <si>
+    <t>https://encrypted-tbn0.gstatic.com/images?q=tbn:ANd9GcQ4u_4e7V1GeVgJl5DU3bjZYZn0ajaiSMhTyw&amp;usqp=CAU</t>
+  </si>
+  <si>
+    <t>60;140</t>
+  </si>
+  <si>
+    <t>100;130</t>
+  </si>
+  <si>
+    <t>90;125</t>
+  </si>
+  <si>
+    <t>100;150</t>
+  </si>
+  <si>
+    <t>40;80</t>
+  </si>
+  <si>
+    <t>https://upload.wikimedia.org/wikipedia/commons/thumb/9/91/Pizza-3007395.jpg/800px-Pizza-3007395.jpg</t>
+  </si>
+  <si>
+    <t>https://www.foodandwine.com/thmb/Wd4lBRZz3X_8qBr69UOu2m7I2iw=/1500x0/filters:no_upscale():max_bytes(150000):strip_icc()/classic-cheese-pizza-FT-RECIPE0422-31a2c938fc2546c9a07b7011658cfd05.jpg</t>
+  </si>
+  <si>
+    <t>https://www.seriouseats.com/thmb/UTE4pHNT6m2WK4sEcVepZ-cpuB4=/1500x0/filters:no_upscale():max_bytes(150000):strip_icc()/spicy-spring-sicilian-pizza-recipe-hero-EDIT-961f7058dcca46a1a057962a4f359b90.jpg</t>
+  </si>
+  <si>
+    <t>https://ooni.com/cdn/shop/articles/20220211142347-margherita-9920_ba86be55-674e-4f35-8094-2067ab41a671.jpg?v=1644590192</t>
+  </si>
+  <si>
+    <t>40;80;100</t>
+  </si>
+  <si>
+    <t>35;80;99</t>
+  </si>
+  <si>
+    <t>40;90;101</t>
+  </si>
+  <si>
+    <t>60;101;129</t>
+  </si>
+  <si>
+    <t>90;100;130</t>
   </si>
 </sst>
 </file>
@@ -523,8 +595,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H6"/>
   <sheetViews>
-    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="C25" sqref="C25"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -533,7 +605,7 @@
     <col min="2" max="2" width="12.88671875" customWidth="1"/>
     <col min="3" max="3" width="10.33203125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="0" hidden="1" customWidth="1"/>
-    <col min="6" max="6" width="63.21875" customWidth="1"/>
+    <col min="6" max="6" width="102" customWidth="1"/>
     <col min="7" max="7" width="44.33203125" customWidth="1"/>
     <col min="8" max="8" width="17.77734375" customWidth="1"/>
   </cols>
@@ -561,7 +633,7 @@
         <v>14</v>
       </c>
       <c r="H1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.3">
@@ -572,13 +644,13 @@
         <v>1000</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>24</v>
+        <v>69</v>
       </c>
       <c r="D2">
         <v>10</v>
       </c>
       <c r="E2" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="F2" s="1" t="s">
         <v>13</v>
@@ -587,7 +659,7 @@
         <v>11</v>
       </c>
       <c r="H2" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.3">
@@ -598,22 +670,22 @@
         <v>1001</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>24</v>
+        <v>70</v>
       </c>
       <c r="D3">
         <v>12</v>
       </c>
       <c r="E3" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>13</v>
+        <v>65</v>
       </c>
       <c r="G3" t="s">
         <v>11</v>
       </c>
       <c r="H3" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.3">
@@ -624,22 +696,22 @@
         <v>1002</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>24</v>
+        <v>71</v>
       </c>
       <c r="D4">
         <v>18</v>
       </c>
       <c r="E4" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>13</v>
+        <v>66</v>
       </c>
       <c r="G4" t="s">
         <v>11</v>
       </c>
       <c r="H4" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.3">
@@ -650,48 +722,48 @@
         <v>1003</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>24</v>
+        <v>72</v>
       </c>
       <c r="D5">
         <v>15</v>
       </c>
       <c r="E5" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>13</v>
+        <v>67</v>
       </c>
       <c r="G5" t="s">
         <v>11</v>
       </c>
       <c r="H5" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B6">
         <v>1004</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>24</v>
+        <v>73</v>
       </c>
       <c r="D6">
         <v>23</v>
       </c>
       <c r="E6" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>13</v>
+        <v>68</v>
       </c>
       <c r="G6" t="s">
         <v>11</v>
       </c>
       <c r="H6" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
   </sheetData>
@@ -712,13 +784,13 @@
   <dimension ref="A1:H7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H1" sqref="H1:H7"/>
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="5" max="5" width="6.88671875" customWidth="1"/>
-    <col min="6" max="6" width="9.21875" customWidth="1"/>
+    <col min="6" max="6" width="67.109375" customWidth="1"/>
     <col min="7" max="7" width="20.88671875" customWidth="1"/>
     <col min="8" max="8" width="12.33203125" customWidth="1"/>
   </cols>
@@ -746,7 +818,7 @@
         <v>14</v>
       </c>
       <c r="H1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.3">
@@ -757,22 +829,22 @@
         <v>2000</v>
       </c>
       <c r="C2" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="D2">
         <v>10</v>
       </c>
       <c r="E2" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>20</v>
+        <v>55</v>
       </c>
       <c r="G2" t="s">
         <v>10</v>
       </c>
       <c r="H2" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.3">
@@ -783,22 +855,22 @@
         <v>2001</v>
       </c>
       <c r="C3" t="s">
-        <v>25</v>
+        <v>60</v>
       </c>
       <c r="D3">
         <v>12</v>
       </c>
       <c r="E3" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>20</v>
+        <v>54</v>
       </c>
       <c r="G3" t="s">
         <v>10</v>
       </c>
       <c r="H3" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.3">
@@ -809,22 +881,22 @@
         <v>2002</v>
       </c>
       <c r="C4" t="s">
-        <v>25</v>
+        <v>61</v>
       </c>
       <c r="D4">
         <v>18</v>
       </c>
       <c r="E4" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>20</v>
+        <v>56</v>
       </c>
       <c r="G4" t="s">
         <v>10</v>
       </c>
       <c r="H4" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.3">
@@ -835,22 +907,22 @@
         <v>2003</v>
       </c>
       <c r="C5" t="s">
-        <v>25</v>
+        <v>62</v>
       </c>
       <c r="D5">
         <v>15</v>
       </c>
       <c r="E5" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>20</v>
+        <v>57</v>
       </c>
       <c r="G5" t="s">
         <v>10</v>
       </c>
       <c r="H5" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.3">
@@ -861,22 +933,22 @@
         <v>2004</v>
       </c>
       <c r="C6" t="s">
-        <v>25</v>
+        <v>63</v>
       </c>
       <c r="D6">
         <v>23</v>
       </c>
       <c r="E6" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>20</v>
+        <v>58</v>
       </c>
       <c r="G6" t="s">
         <v>10</v>
       </c>
       <c r="H6" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.3">
@@ -887,22 +959,22 @@
         <v>2005</v>
       </c>
       <c r="C7" t="s">
-        <v>25</v>
+        <v>64</v>
       </c>
       <c r="D7">
         <v>30</v>
       </c>
       <c r="E7" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>20</v>
+        <v>59</v>
       </c>
       <c r="G7" t="s">
         <v>10</v>
       </c>
       <c r="H7" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
   </sheetData>
@@ -910,6 +982,11 @@
   <hyperlinks>
     <hyperlink ref="F2" r:id="rId1" xr:uid="{1AE3C984-612A-46CD-AA73-3F57EF51D33B}"/>
     <hyperlink ref="F3:F7" r:id="rId2" display="https://idsb.tmgrup.com.tr/ly/uploads/images/2023/01/15/251807.jpg" xr:uid="{FE0273D9-6768-45B6-AD5A-F7BE80F56216}"/>
+    <hyperlink ref="F3" r:id="rId3" xr:uid="{EFAA2761-EC69-435D-B5C7-CB9865894976}"/>
+    <hyperlink ref="F4" r:id="rId4" xr:uid="{E51F2D0A-2A11-4484-A0A5-68AB088DAB64}"/>
+    <hyperlink ref="F5" r:id="rId5" xr:uid="{C0A99FDB-E690-4B40-89F2-DF49A72F21F6}"/>
+    <hyperlink ref="F6" r:id="rId6" xr:uid="{8A518579-82C0-4466-A73A-708DF701605A}"/>
+    <hyperlink ref="F7" r:id="rId7" xr:uid="{1A37CB52-7A5B-4969-91CD-E6FD1E552618}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -920,7 +997,7 @@
   <dimension ref="A1:F6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -947,107 +1024,107 @@
         <v>9</v>
       </c>
       <c r="F1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>45</v>
+        <v>49</v>
       </c>
       <c r="B2">
         <v>3000</v>
       </c>
       <c r="C2">
-        <v>50</v>
+        <v>20</v>
       </c>
       <c r="D2" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="F2" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>46</v>
+        <v>50</v>
       </c>
       <c r="B3">
         <v>3001</v>
       </c>
       <c r="C3">
-        <v>50</v>
+        <v>80</v>
       </c>
       <c r="D3" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>21</v>
+        <v>43</v>
       </c>
       <c r="F3" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="B4">
         <v>3002</v>
       </c>
       <c r="C4">
-        <v>50</v>
+        <v>40</v>
       </c>
       <c r="D4" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>21</v>
+        <v>44</v>
       </c>
       <c r="F4" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>48</v>
+        <v>52</v>
       </c>
       <c r="B5">
         <v>3003</v>
       </c>
       <c r="C5">
-        <v>50</v>
+        <v>30</v>
       </c>
       <c r="D5" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>21</v>
+        <v>45</v>
       </c>
       <c r="F5" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>49</v>
+        <v>53</v>
       </c>
       <c r="B6">
         <v>3004</v>
       </c>
-      <c r="C6">
-        <v>50</v>
+      <c r="C6" t="s">
+        <v>47</v>
       </c>
       <c r="D6" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>21</v>
+        <v>46</v>
       </c>
       <c r="F6" t="s">
-        <v>31</v>
+        <v>48</v>
       </c>
     </row>
   </sheetData>
@@ -1055,6 +1132,10 @@
   <hyperlinks>
     <hyperlink ref="E2" r:id="rId1" xr:uid="{1D0A74C3-2AF4-4599-900C-BD3440757B3F}"/>
     <hyperlink ref="E3:E6" r:id="rId2" display="https://src.zakaz.atbmarket.com/cache/photos/37541/catalog_list_37541.jpg" xr:uid="{00DCE022-8DFA-4974-8CFC-E6F8CD169239}"/>
+    <hyperlink ref="E3" r:id="rId3" xr:uid="{DAD50415-C9A2-44F1-955B-51668212B919}"/>
+    <hyperlink ref="E4" r:id="rId4" xr:uid="{EC2AE491-1941-4CE1-B129-556101B0F94B}"/>
+    <hyperlink ref="E5" r:id="rId5" xr:uid="{F2785982-EA58-4E1F-8E3A-5AACBF5C40F0}"/>
+    <hyperlink ref="E6" r:id="rId6" xr:uid="{4CE3DA4C-3065-442B-9124-03EE012F3687}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1064,8 +1145,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B45BDF59-3489-4E08-8326-3D9E2299AB64}">
   <dimension ref="A1:B10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:B10"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1078,7 +1159,7 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="B1" t="s">
         <v>5</v>
@@ -1086,74 +1167,74 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B2" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B3" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B4" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B5" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B6" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B7" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B8" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B9" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B10" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
     </row>
   </sheetData>

</xml_diff>